<commit_message>
Calibrate Georgia for total population
</commit_message>
<xml_diff>
--- a/autumn/xls/data_georgia.xlsx
+++ b/autumn/xls/data_georgia.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rragonnet\Google Drive\GitHub\AuTuMN\autumn\xls\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="795" windowWidth="20370" windowHeight="7050" tabRatio="807"/>
+    <workbookView xWindow="120" yWindow="792" windowWidth="20376" windowHeight="7056" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="4" r:id="rId1"/>
     <sheet name="time_variants" sheetId="2" r:id="rId2"/>
     <sheet name="dropdown_lists" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -1668,6 +1673,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1715,7 +1723,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1750,7 +1758,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1962,17 +1970,17 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="51.28515625" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="93.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="93.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>6</v>
       </c>
@@ -1989,7 +1997,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
@@ -2006,7 +2014,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>17</v>
       </c>
@@ -2019,12 +2027,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="15">
-        <v>4000000</v>
+        <v>3700000</v>
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="16"/>
@@ -2032,7 +2040,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>21</v>
       </c>
@@ -2071,31 +2079,31 @@
       <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="56" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="2" customWidth="1"/>
-    <col min="4" max="5" width="7.42578125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="7.44140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="1" customWidth="1"/>
-    <col min="8" max="9" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="7.42578125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.140625" style="1" customWidth="1"/>
-    <col min="19" max="20" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.44140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.6640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="7.33203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="7.44140625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.109375" style="1" customWidth="1"/>
+    <col min="19" max="20" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="8" style="1" customWidth="1"/>
-    <col min="24" max="24" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.85546875" style="1" customWidth="1"/>
-    <col min="28" max="16384" width="9.140625" style="1"/>
+    <col min="24" max="24" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.88671875" style="1" customWidth="1"/>
+    <col min="28" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -2205,7 +2213,7 @@
       <selection activeCell="D4" sqref="A2:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">

</xml_diff>